<commit_message>
deleting visualizacion diferenciada section
</commit_message>
<xml_diff>
--- a/datasets/merge_william.xlsx
+++ b/datasets/merge_william.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,6 +508,11 @@
           <t>diff</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>% aplazado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -584,6 +589,9 @@
       <c r="N2" t="n">
         <v>68343460000</v>
       </c>
+      <c r="O2" t="n">
+        <v>82.09999999999999</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -651,6 +659,9 @@
       <c r="N3" t="n">
         <v>510258000000</v>
       </c>
+      <c r="O3" t="n">
+        <v>16.4</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -717,6 +728,9 @@
       <c r="N4" t="n">
         <v>3644790032592</v>
       </c>
+      <c r="O4" t="n">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -783,6 +797,9 @@
       <c r="N5" t="n">
         <v>5579384497</v>
       </c>
+      <c r="O5" t="n">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -849,6 +866,9 @@
       <c r="N6" t="n">
         <v>26971314402</v>
       </c>
+      <c r="O6" t="n">
+        <v>11.3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -915,6 +935,9 @@
       <c r="N7" t="n">
         <v>2595107018509</v>
       </c>
+      <c r="O7" t="n">
+        <v>4.9</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -980,6 +1003,9 @@
       </c>
       <c r="N8" t="n">
         <v>2049876578249</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="9">
@@ -1057,6 +1083,9 @@
       <c r="N9" t="n">
         <v>0</v>
       </c>
+      <c r="O9" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1129,6 +1158,9 @@
       <c r="N10" t="n">
         <v>36340895394</v>
       </c>
+      <c r="O10" t="n">
+        <v>80.7</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1197,6 +1229,9 @@
       </c>
       <c r="N11" t="n">
         <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -1267,6 +1302,9 @@
       <c r="N12" t="n">
         <v>21000000000</v>
       </c>
+      <c r="O12" t="n">
+        <v>19.2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1338,6 +1376,9 @@
       <c r="N13" t="n">
         <v>37561316512</v>
       </c>
+      <c r="O13" t="n">
+        <v>28.5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1407,6 +1448,9 @@
       <c r="N14" t="n">
         <v>0</v>
       </c>
+      <c r="O14" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1476,6 +1520,9 @@
       </c>
       <c r="N15" t="n">
         <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="16">
@@ -1555,6 +1602,9 @@
       <c r="N16" t="n">
         <v>175466477273</v>
       </c>
+      <c r="O16" t="n">
+        <v>1.1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1629,6 +1679,9 @@
       <c r="N17" t="n">
         <v>6500000000</v>
       </c>
+      <c r="O17" t="n">
+        <v>18.8</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1699,6 +1752,9 @@
       </c>
       <c r="N18" t="n">
         <v>68166193182</v>
+      </c>
+      <c r="O18" t="n">
+        <v>4.2</v>
       </c>
     </row>
     <row r="19">
@@ -1777,6 +1833,9 @@
       <c r="N19" t="n">
         <v>16000000000</v>
       </c>
+      <c r="O19" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1854,6 +1913,9 @@
       <c r="N20" t="n">
         <v>52200000000</v>
       </c>
+      <c r="O20" t="n">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1928,6 +1990,9 @@
       <c r="N21" t="n">
         <v>12116619318</v>
       </c>
+      <c r="O21" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1999,6 +2064,9 @@
       <c r="N22" t="n">
         <v>8000000000</v>
       </c>
+      <c r="O22" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2071,6 +2139,9 @@
       <c r="N23" t="n">
         <v>0</v>
       </c>
+      <c r="O23" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2142,6 +2213,9 @@
       </c>
       <c r="N24" t="n">
         <v>233800000000</v>
+      </c>
+      <c r="O24" t="n">
+        <v>43.7</v>
       </c>
     </row>
     <row r="25">
@@ -2215,6 +2289,9 @@
       </c>
       <c r="N25" t="n">
         <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="26">
@@ -2291,6 +2368,9 @@
       <c r="N26" t="n">
         <v>6000000000</v>
       </c>
+      <c r="O26" t="n">
+        <v>14.3</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2364,6 +2444,9 @@
       <c r="N27" t="n">
         <v>15700000000</v>
       </c>
+      <c r="O27" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2436,6 +2519,9 @@
       <c r="N28" t="n">
         <v>24000000000</v>
       </c>
+      <c r="O28" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2506,6 +2592,9 @@
       </c>
       <c r="N29" t="n">
         <v>268575063057</v>
+      </c>
+      <c r="O29" t="n">
+        <v>15.7</v>
       </c>
     </row>
     <row r="30">
@@ -2581,6 +2670,9 @@
       <c r="N30" t="n">
         <v>0</v>
       </c>
+      <c r="O30" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2649,6 +2741,9 @@
       </c>
       <c r="N31" t="n">
         <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="32">
@@ -2723,6 +2818,9 @@
       <c r="N32" t="n">
         <v>0</v>
       </c>
+      <c r="O32" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2795,6 +2893,9 @@
       <c r="N33" t="n">
         <v>332338635846</v>
       </c>
+      <c r="O33" t="n">
+        <v>69.90000000000001</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2865,6 +2966,9 @@
       <c r="N34" t="n">
         <v>0</v>
       </c>
+      <c r="O34" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2936,6 +3040,9 @@
       <c r="N35" t="n">
         <v>0</v>
       </c>
+      <c r="O35" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3007,6 +3114,9 @@
       <c r="N36" t="n">
         <v>0</v>
       </c>
+      <c r="O36" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3078,6 +3188,9 @@
       <c r="N37" t="n">
         <v>0</v>
       </c>
+      <c r="O37" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3132,6 +3245,7 @@
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3186,6 +3300,7 @@
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3240,6 +3355,7 @@
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3306,6 +3422,9 @@
       </c>
       <c r="N41" t="n">
         <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="42">
@@ -3376,6 +3495,9 @@
       <c r="N42" t="n">
         <v>0</v>
       </c>
+      <c r="O42" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3445,6 +3567,9 @@
       <c r="N43" t="n">
         <v>154987000000</v>
       </c>
+      <c r="O43" t="n">
+        <v>30.1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3512,6 +3637,9 @@
       <c r="N44" t="n">
         <v>36349259000</v>
       </c>
+      <c r="O44" t="n">
+        <v>24.6</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3579,6 +3707,9 @@
       <c r="N45" t="n">
         <v>85012469000</v>
       </c>
+      <c r="O45" t="n">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3643,6 +3774,9 @@
       <c r="N46" t="n">
         <v>0</v>
       </c>
+      <c r="O46" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3708,6 +3842,9 @@
       <c r="N47" t="n">
         <v>8947653333</v>
       </c>
+      <c r="O47" t="n">
+        <v>66.8</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3773,6 +3910,9 @@
       <c r="N48" t="n">
         <v>0</v>
       </c>
+      <c r="O48" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3837,6 +3977,9 @@
       </c>
       <c r="N49" t="n">
         <v>15000000000</v>
+      </c>
+      <c r="O49" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="50">
@@ -3905,6 +4048,9 @@
       <c r="N50" t="n">
         <v>0</v>
       </c>
+      <c r="O50" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3969,6 +4115,9 @@
       <c r="N51" t="n">
         <v>0</v>
       </c>
+      <c r="O51" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4031,6 +4180,9 @@
       </c>
       <c r="N52" t="n">
         <v>67408509000</v>
+      </c>
+      <c r="O52" t="n">
+        <v>15.1</v>
       </c>
     </row>
     <row r="53">
@@ -4098,6 +4250,9 @@
       <c r="N53" t="n">
         <v>216754750000</v>
       </c>
+      <c r="O53" t="n">
+        <v>4.4</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4160,6 +4315,9 @@
       </c>
       <c r="N54" t="n">
         <v>51511000000</v>
+      </c>
+      <c r="O54" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="55">
@@ -4224,6 +4382,9 @@
       </c>
       <c r="N55" t="n">
         <v>300899600000</v>
+      </c>
+      <c r="O55" t="n">
+        <v>51.1</v>
       </c>
     </row>
     <row r="56">
@@ -4290,6 +4451,9 @@
       <c r="N56" t="n">
         <v>1200000000</v>
       </c>
+      <c r="O56" t="n">
+        <v>46.3</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4355,6 +4519,9 @@
       <c r="N57" t="n">
         <v>1035000000</v>
       </c>
+      <c r="O57" t="n">
+        <v>53.7</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4420,6 +4587,9 @@
       <c r="N58" t="n">
         <v>1259000000</v>
       </c>
+      <c r="O58" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4484,6 +4654,9 @@
       <c r="N59" t="n">
         <v>74128000000</v>
       </c>
+      <c r="O59" t="n">
+        <v>52.4</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4548,6 +4721,9 @@
       <c r="N60" t="n">
         <v>3264000000</v>
       </c>
+      <c r="O60" t="n">
+        <v>94.8</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4612,6 +4788,9 @@
       <c r="N61" t="n">
         <v>0</v>
       </c>
+      <c r="O61" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4676,6 +4855,9 @@
       <c r="N62" t="n">
         <v>0</v>
       </c>
+      <c r="O62" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4740,6 +4922,9 @@
       <c r="N63" t="n">
         <v>5216716605874</v>
       </c>
+      <c r="O63" t="n">
+        <v>18.3</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4804,6 +4989,9 @@
       <c r="N64" t="n">
         <v>0</v>
       </c>
+      <c r="O64" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4868,6 +5056,9 @@
       <c r="N65" t="n">
         <v>0</v>
       </c>
+      <c r="O65" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4932,6 +5123,9 @@
       <c r="N66" t="n">
         <v>0</v>
       </c>
+      <c r="O66" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4996,6 +5190,9 @@
       <c r="N67" t="n">
         <v>0</v>
       </c>
+      <c r="O67" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5060,6 +5257,9 @@
       <c r="N68" t="n">
         <v>0</v>
       </c>
+      <c r="O68" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5124,6 +5324,9 @@
       <c r="N69" t="n">
         <v>325464110000</v>
       </c>
+      <c r="O69" t="n">
+        <v>38.1</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5188,6 +5391,9 @@
       <c r="N70" t="n">
         <v>0</v>
       </c>
+      <c r="O70" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5252,6 +5458,9 @@
       <c r="N71" t="n">
         <v>4000000000</v>
       </c>
+      <c r="O71" t="n">
+        <v>71.40000000000001</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5316,6 +5525,9 @@
       <c r="N72" t="n">
         <v>0</v>
       </c>
+      <c r="O72" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5380,6 +5592,9 @@
       <c r="N73" t="n">
         <v>0</v>
       </c>
+      <c r="O73" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5444,6 +5659,9 @@
       <c r="N74" t="n">
         <v>0</v>
       </c>
+      <c r="O74" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -5508,6 +5726,9 @@
       <c r="N75" t="n">
         <v>166829900000</v>
       </c>
+      <c r="O75" t="n">
+        <v>16.6</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -5572,6 +5793,9 @@
       <c r="N76" t="n">
         <v>0</v>
       </c>
+      <c r="O76" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5636,6 +5860,9 @@
       <c r="N77" t="n">
         <v>0</v>
       </c>
+      <c r="O77" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -5700,6 +5927,9 @@
       <c r="N78" t="n">
         <v>0</v>
       </c>
+      <c r="O78" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -5764,6 +5994,9 @@
       <c r="N79" t="n">
         <v>0</v>
       </c>
+      <c r="O79" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -5828,6 +6061,9 @@
       <c r="N80" t="n">
         <v>0</v>
       </c>
+      <c r="O80" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -5892,6 +6128,9 @@
       <c r="N81" t="n">
         <v>0</v>
       </c>
+      <c r="O81" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -5956,6 +6195,9 @@
       <c r="N82" t="n">
         <v>0</v>
       </c>
+      <c r="O82" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -6020,6 +6262,9 @@
       </c>
       <c r="N83" t="n">
         <v>15006000000</v>
+      </c>
+      <c r="O83" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="84">
@@ -6089,6 +6334,9 @@
       </c>
       <c r="N84" t="n">
         <v>0</v>
+      </c>
+      <c r="O84" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="85">
@@ -6158,6 +6406,9 @@
       <c r="N85" t="n">
         <v>27059460798000</v>
       </c>
+      <c r="O85" t="n">
+        <v>9.300000000000001</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -6225,6 +6476,9 @@
       <c r="N86" t="n">
         <v>123451000000</v>
       </c>
+      <c r="O86" t="n">
+        <v>43.2</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6289,6 +6543,9 @@
       </c>
       <c r="N87" t="n">
         <v>200000000000</v>
+      </c>
+      <c r="O87" t="n">
+        <v>25.6</v>
       </c>
     </row>
     <row r="88">
@@ -6358,6 +6615,9 @@
       <c r="N88" t="n">
         <v>100000000000</v>
       </c>
+      <c r="O88" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6420,6 +6680,9 @@
       <c r="N89" t="n">
         <v>2684217000</v>
       </c>
+      <c r="O89" t="n">
+        <v>65.09999999999999</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -6482,6 +6745,9 @@
       <c r="N90" t="n">
         <v>10769569000</v>
       </c>
+      <c r="O90" t="n">
+        <v>48.1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -6544,6 +6810,9 @@
       <c r="N91" t="n">
         <v>5647256000</v>
       </c>
+      <c r="O91" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -6607,6 +6876,9 @@
       </c>
       <c r="N92" t="n">
         <v>5259000000</v>
+      </c>
+      <c r="O92" t="n">
+        <v>27.6</v>
       </c>
     </row>
     <row r="93">
@@ -6674,6 +6946,9 @@
       <c r="N93" t="n">
         <v>160201053000</v>
       </c>
+      <c r="O93" t="n">
+        <v>3.6</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -6736,6 +7011,9 @@
       </c>
       <c r="N94" t="n">
         <v>448700000000</v>
+      </c>
+      <c r="O94" t="n">
+        <v>27.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>